<commit_message>
Some small changes and tests added
</commit_message>
<xml_diff>
--- a/shorty_entries.xlsx
+++ b/shorty_entries.xlsx
@@ -12,36 +12,75 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
-    <t>www.youtube.com</t>
+    <t>www.google.com</t>
   </si>
   <si>
-    <t>co8uvt6l</t>
+    <t>khk9gs3t</t>
   </si>
   <si>
     <t>www.facebook.com</t>
   </si>
   <si>
-    <t>xkq8vjqv</t>
-  </si>
-  <si>
-    <t>xy2id582</t>
+    <t>n1c2cvoh</t>
   </si>
   <si>
     <t>www.riteh.hr</t>
   </si>
   <si>
-    <t>fbklaopz</t>
+    <t>ec1lybi8</t>
   </si>
   <si>
-    <t>0v2ffdc7</t>
+    <t>7f8ps11s</t>
   </si>
   <si>
-    <t>www.kkso.com</t>
+    <t>www.youtube.com</t>
   </si>
   <si>
-    <t>ayz51beq</t>
+    <t>a9dgoy08</t>
+  </si>
+  <si>
+    <t>www.links.hr</t>
+  </si>
+  <si>
+    <t>ptfif9wn</t>
+  </si>
+  <si>
+    <t>zep7anp7</t>
+  </si>
+  <si>
+    <t>2d2qh4pn</t>
+  </si>
+  <si>
+    <t>xinblroi</t>
+  </si>
+  <si>
+    <t>75ewbs47</t>
+  </si>
+  <si>
+    <t>n3098j0g</t>
+  </si>
+  <si>
+    <t>37w8pj6m</t>
+  </si>
+  <si>
+    <t>5tkkcopb</t>
+  </si>
+  <si>
+    <t>v6zhob9m</t>
+  </si>
+  <si>
+    <t>www.hjdsahldkjhsajlkdhljsakdhsajkldhjsadhjsahdjkalshdjklhsakjldas.com</t>
+  </si>
+  <si>
+    <t>1hmy6atg</t>
+  </si>
+  <si>
+    <t>www.hdsjkad.com</t>
+  </si>
+  <si>
+    <t>jco2hmrs</t>
   </si>
 </sst>
 </file>
@@ -97,10 +136,10 @@
         <v>0.0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2">
@@ -111,7 +150,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3">
@@ -119,10 +158,10 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running version of shorty app
</commit_message>
<xml_diff>
--- a/shorty_entries.xlsx
+++ b/shorty_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krusv\IdeaProjects\shorty-asee-internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F6B175-9F91-4BB0-86DE-3B06D894D389}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BC58A7-7F72-49FA-AA51-DB2AFEB9A3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
-  <si>
-    <t>www.google.com</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>www.riteh.hr</t>
   </si>
@@ -31,70 +28,22 @@
     <t>www.youtube.com</t>
   </si>
   <si>
-    <t>37w8pj6m</t>
-  </si>
-  <si>
-    <t>v6zhob9m</t>
-  </si>
-  <si>
-    <t>bw6hlpf4</t>
-  </si>
-  <si>
-    <t>https://www.google.com/url?sa=i&amp;url=https%3A%2F%2Fwww.dovido.hr%2FSlike-prirode-i-krajolika%2FSlika-carobno-staklo-usred-planina&amp;psig=AOvVaw2sYqDirwZBXeSzGiu4wXBn&amp;ust=1685130887944000&amp;source=images&amp;cd=vfe&amp;ved=0CBEQjRxqFwoTCPjx5vCfkf8CFQAAAAAdAAAAABAE</t>
-  </si>
-  <si>
-    <t>fxt5ucea</t>
-  </si>
-  <si>
-    <t>mj4uik9f</t>
-  </si>
-  <si>
-    <t>www.links.hr</t>
-  </si>
-  <si>
-    <t>u092hubf</t>
-  </si>
-  <si>
-    <t>aqfz6yhk</t>
-  </si>
-  <si>
     <t>www.facebook.com</t>
   </si>
   <si>
     <t>npblgmap</t>
   </si>
   <si>
-    <t>www-links-hr</t>
-  </si>
-  <si>
-    <t>qxznojp0</t>
-  </si>
-  <si>
-    <t>3dec7m2s</t>
-  </si>
-  <si>
-    <t>5cm6f1jf</t>
-  </si>
-  <si>
-    <t>6o0xbnyd</t>
-  </si>
-  <si>
-    <t>fznrirpj</t>
-  </si>
-  <si>
-    <t>www.kiko.com</t>
-  </si>
-  <si>
-    <t>nkzi7bhk</t>
-  </si>
-  <si>
-    <t>iygyow7z</t>
-  </si>
-  <si>
     <t>unvk4d1q</t>
   </si>
   <si>
-    <t>iaup71ou</t>
+    <t>nk2dari7</t>
+  </si>
+  <si>
+    <t>https://www.google.com/maps</t>
+  </si>
+  <si>
+    <t>lykknxr3</t>
   </si>
 </sst>
 </file>
@@ -447,35 +396,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" bestFit="true" customWidth="true" width="255.7109375"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="n" s="0">
-        <v>0.0</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="0">
+        <v>0</v>
       </c>
       <c r="B1" t="s" s="0">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s" s="0">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="n" s="0">
-        <v>1.0</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="0">
+        <v>1</v>
       </c>
       <c r="B2" t="s" s="0">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="0">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="C2" t="s" s="0">
-        <v>23</v>
+      <c r="C3" t="s" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing errors and adding configuration files
</commit_message>
<xml_diff>
--- a/shorty_entries.xlsx
+++ b/shorty_entries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krusv\IdeaProjects\shorty-asee-internship\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BC58A7-7F72-49FA-AA51-DB2AFEB9A3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5468B378-4CAA-42AC-9A73-B674777C548B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9600" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -20,37 +20,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>www.riteh.hr</t>
+    <t>https://www.baeldung.com/properties-with-spring</t>
   </si>
   <si>
-    <t>www.youtube.com</t>
+    <t>dnc29h4a</t>
   </si>
   <si>
-    <t>www.facebook.com</t>
+    <t>www.google.com</t>
   </si>
   <si>
-    <t>npblgmap</t>
-  </si>
-  <si>
-    <t>unvk4d1q</t>
-  </si>
-  <si>
-    <t>nk2dari7</t>
-  </si>
-  <si>
-    <t>https://www.google.com/maps</t>
-  </si>
-  <si>
-    <t>lykknxr3</t>
+    <t>7nm7eid9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -396,59 +383,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="255.7109375"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="0">
+      <c r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="0">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s" s="0">
-        <v>3</v>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="0">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="0">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s" s="0">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>7</v>
+      <c r="C2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>